<commit_message>
add new samples form opj
</commit_message>
<xml_diff>
--- a/!_chains/chain table.xlsx
+++ b/!_chains/chain table.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,7 +384,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>RoZF</t>
+          <t>Ro_tot</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -394,12 +394,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>#ser</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>#par</t>
+          <t>Npar</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -415,6 +415,36 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>status</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>wp</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Iab</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Ej</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Ec</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Ro</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rn</t>
         </is>
       </c>
     </row>
@@ -454,6 +484,22 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L2" t="n">
+        <v>4.655535216483947</v>
+      </c>
+      <c r="M2" t="n">
+        <v>6.113064250538915e-07</v>
+      </c>
+      <c r="N2" t="n">
+        <v>14.57174614458185</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>465</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -465,7 +511,7 @@
         <v>0.001675</v>
       </c>
       <c r="C3" t="n">
-        <v>115200</v>
+        <v>115000</v>
       </c>
       <c r="D3" t="n">
         <v>1.53e-10</v>
@@ -495,6 +541,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L3" t="n">
+        <v>1.323921302708037</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4.943608480870601e-08</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.178410775170532</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P3" t="n">
+        <v>50300</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>5750</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -506,7 +570,7 @@
         <v>0.001875</v>
       </c>
       <c r="C4" t="n">
-        <v>84380</v>
+        <v>84300</v>
       </c>
       <c r="D4" t="n">
         <v>1.98e-09</v>
@@ -536,6 +600,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L4" t="n">
+        <v>1.546312630051307</v>
+      </c>
+      <c r="M4" t="n">
+        <v>6.74394988493617e-08</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.607559183210097</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3941.5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>4215</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -547,7 +629,7 @@
         <v>0.0002178</v>
       </c>
       <c r="C5" t="n">
-        <v>8756</v>
+        <v>8750</v>
       </c>
       <c r="D5" t="n">
         <v>3.9e-09</v>
@@ -577,6 +659,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L5" t="n">
+        <v>1.517773842791293</v>
+      </c>
+      <c r="M5" t="n">
+        <v>6.497314003429933e-08</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.548768447366985</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P5" t="n">
+        <v>657</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4375</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -588,19 +688,19 @@
         <v>0.001385</v>
       </c>
       <c r="C6" t="n">
-        <v>1754000</v>
+        <v>1800000</v>
       </c>
       <c r="D6" t="n">
-        <v>3.2e-13</v>
+        <v>3.1e-13</v>
       </c>
       <c r="E6" t="n">
-        <v>236700000</v>
+        <v>200000000</v>
       </c>
       <c r="F6" t="n">
         <v>903200000</v>
       </c>
       <c r="G6" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
@@ -615,8 +715,26 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>fabd</t>
-        </is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0.2993090382218327</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.526733223556085e-09</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.06022988406427163</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P6" t="n">
+        <v>12500000</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>112500</v>
       </c>
     </row>
     <row r="7">
@@ -629,7 +747,7 @@
         <v>0.002495</v>
       </c>
       <c r="C7" t="n">
-        <v>993500</v>
+        <v>993000</v>
       </c>
       <c r="D7" t="n">
         <v>2.1e-11</v>
@@ -659,6 +777,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L7" t="n">
+        <v>0.4505432279086851</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5.72522633736273e-09</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1364725469734251</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P7" t="n">
+        <v>215950</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>49650</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -670,13 +806,13 @@
         <v>0.003345</v>
       </c>
       <c r="C8" t="n">
-        <v>664700</v>
+        <v>726000</v>
       </c>
       <c r="D8" t="n">
         <v>1.2e-12</v>
       </c>
       <c r="E8" t="n">
-        <v>22920000</v>
+        <v>28000000</v>
       </c>
       <c r="F8" t="n">
         <v>958700000</v>
@@ -697,8 +833,26 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>fabd</t>
-        </is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0.5269176910920534</v>
+      </c>
+      <c r="M8" t="n">
+        <v>7.830784783748197e-09</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1866628638355526</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1400000</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>36300</v>
       </c>
     </row>
     <row r="9">
@@ -711,13 +865,13 @@
         <v>0.0003186</v>
       </c>
       <c r="C9" t="n">
-        <v>119900</v>
+        <v>122000</v>
       </c>
       <c r="D9" t="n">
-        <v>2.68e-12</v>
+        <v>2.5e-12</v>
       </c>
       <c r="E9" t="n">
-        <v>29090000</v>
+        <v>28000000</v>
       </c>
       <c r="F9" t="n">
         <v>920900000</v>
@@ -738,8 +892,26 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>fabd</t>
-        </is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0.5748389308445906</v>
+      </c>
+      <c r="M9" t="n">
+        <v>9.319917627870805e-09</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2221594084337888</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P9" t="n">
+        <v>7000000</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>30500</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +924,7 @@
         <v>0.00501</v>
       </c>
       <c r="C10" t="n">
-        <v>594200</v>
+        <v>594000</v>
       </c>
       <c r="D10" t="n">
         <v>2e-11</v>
@@ -782,6 +954,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L10" t="n">
+        <v>0.7134499264189915</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.435643877020503e-08</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.3422152503651797</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P10" t="n">
+        <v>257166.6666666667</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>19800</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -793,7 +983,7 @@
         <v>0.00307</v>
       </c>
       <c r="C11" t="n">
-        <v>585900</v>
+        <v>585000</v>
       </c>
       <c r="D11" t="n">
         <v>2.2e-11</v>
@@ -823,6 +1013,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L11" t="n">
+        <v>0.07939110757275286</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.457730705897741e-08</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.3474801003707979</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P11" t="n">
+        <v>8833.333333333334</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>19500</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -834,7 +1042,7 @@
         <v>0.00172</v>
       </c>
       <c r="C12" t="n">
-        <v>66130</v>
+        <v>66100</v>
       </c>
       <c r="D12" t="n">
         <v>5.4e-09</v>
@@ -864,6 +1072,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L12" t="n">
+        <v>2.138730142415677</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.29012475484142e-07</v>
+      </c>
+      <c r="N12" t="n">
+        <v>3.075277741556986</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P12" t="n">
+        <v>28.36666666666667</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2203.333333333333</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -873,7 +1099,7 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>168200</v>
+        <v>168000</v>
       </c>
       <c r="D13" t="n">
         <v>1.6e-10</v>
@@ -901,6 +1127,24 @@
           <t>measd</t>
         </is>
       </c>
+      <c r="L13" t="n">
+        <v>0.1047563010599542</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2.538013282589817e-08</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.6049876747527285</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1582</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>11200</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -912,7 +1156,7 @@
         <v>0.0001645</v>
       </c>
       <c r="C14" t="n">
-        <v>1458</v>
+        <v>1450</v>
       </c>
       <c r="D14" t="n">
         <v>1.37e-07</v>
@@ -940,6 +1184,24 @@
           <t>measd</t>
         </is>
       </c>
+      <c r="L14" t="n">
+        <v>0.3009666907808027</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.960396466552135e-07</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4.673008246365902</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.002422982803154429</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -951,7 +1213,7 @@
         <v>0.002021</v>
       </c>
       <c r="C15" t="n">
-        <v>23350</v>
+        <v>23300</v>
       </c>
       <c r="D15" t="n">
         <v>5.6e-09</v>
@@ -979,6 +1241,24 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L15" t="n">
+        <v>0.2907837300758601</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.829983826073345e-07</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4.362142890920961</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.002422982803154429</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-20.46666666666667</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1553.333333333333</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1018,6 +1298,24 @@
           <t>measd</t>
         </is>
       </c>
+      <c r="L16" t="n">
+        <v>0.3801228586647764</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1.895049917667064e-07</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4.517241304820373</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.00399838579370588</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1029,7 +1327,7 @@
         <v>0.001931</v>
       </c>
       <c r="C17" t="n">
-        <v>254200</v>
+        <v>254000</v>
       </c>
       <c r="D17" t="n">
         <v>3.71e-11</v>
@@ -1057,6 +1355,24 @@
           <t>measd</t>
         </is>
       </c>
+      <c r="L17" t="n">
+        <v>0.085195751409178</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1.678685950689328e-08</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.400149328182907</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P17" t="n">
+        <v>666.6666666666666</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>16933.33333333333</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1096,6 +1412,24 @@
           <t>measd</t>
         </is>
       </c>
+      <c r="L18" t="n">
+        <v>0.08578886673568814</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.702140644611135e-08</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.4057402369599137</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P18" t="n">
+        <v>100000</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>16700</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1134,6 +1468,24 @@
         <is>
           <t>fabd</t>
         </is>
+      </c>
+      <c r="L19" t="n">
+        <v>0.07035122392769246</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.1446610240942e-08</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.2728535016334454</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P19" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>24833.33333333333</v>
       </c>
     </row>
     <row r="20">
@@ -1170,6 +1522,22 @@
           <t>fabd</t>
         </is>
       </c>
+      <c r="L20" t="n">
+        <v>0.5083511251357323</v>
+      </c>
+      <c r="M20" t="n">
+        <v>4.373192117693223e-09</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.1042440301112394</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.3098748990122057</v>
+      </c>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="n">
+        <v>65000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1208,6 +1576,214 @@
         <is>
           <t>fabd</t>
         </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0.04551345373112418</v>
+      </c>
+      <c r="M21" t="n">
+        <v>4.790856533427969e-09</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.1141999206274813</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.002267377309845408</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1666666.666666667</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>59333.33333333334</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>D060B2N7</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>148000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.6e-12</v>
+      </c>
+      <c r="E22" t="n">
+        <v>41000000</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>7.682634801352961e-09</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.1831314042494746</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>10250000</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>D059BBN4</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>2300000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.2e-13</v>
+      </c>
+      <c r="E23" t="n">
+        <v>217000000</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>4e-14</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0.2960378029715247</v>
+      </c>
+      <c r="M23" t="n">
+        <v>2.4718042404353e-09</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.0589205387585266</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P23" t="n">
+        <v>10850000</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>D059BBN7</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.1e-13</v>
+      </c>
+      <c r="E24" t="n">
+        <v>190000000</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>19</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>4e-14</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>0.3019696153291183</v>
+      </c>
+      <c r="M24" t="n">
+        <v>2.571853459691015e-09</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.06130541770827649</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P24" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>110526.3157894737</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>D059BBN3</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.9e-13</v>
+      </c>
+      <c r="E25" t="n">
+        <v>87000000</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>20</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>4e-14</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>measd_lv</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>0.3098142883151567</v>
+      </c>
+      <c r="M25" t="n">
+        <v>2.707214168095805e-09</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.06453201864029104</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.1859249394073234</v>
+      </c>
+      <c r="P25" t="n">
+        <v>4350000</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>105000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update number of SQUIDs
</commit_message>
<xml_diff>
--- a/!_chains/chain table.xlsx
+++ b/!_chains/chain table.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\racco\Documents\QCoDes\measDC\!_chains\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D893BEDD-D4F7-4C2E-9432-5B64D567867C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="907" yWindow="-98" windowWidth="19710" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -112,81 +118,82 @@
     <t>D078N5</t>
   </si>
   <si>
+    <t>D059BBN2_n</t>
+  </si>
+  <si>
+    <t>D059BBN8</t>
+  </si>
+  <si>
+    <t>D053N2</t>
+  </si>
+  <si>
+    <t>D053N4</t>
+  </si>
+  <si>
+    <t>D053N7</t>
+  </si>
+  <si>
+    <t>D055B1N2</t>
+  </si>
+  <si>
+    <t>D055B1N4</t>
+  </si>
+  <si>
+    <t>D055B1N5</t>
+  </si>
+  <si>
+    <t>D057B1N6</t>
+  </si>
+  <si>
+    <t>D057B1N7</t>
+  </si>
+  <si>
+    <t>D057B1N8</t>
+  </si>
+  <si>
+    <t>D057B1N9</t>
+  </si>
+  <si>
+    <t>D059B6N5</t>
+  </si>
+  <si>
+    <t>D059B6N7</t>
+  </si>
+  <si>
+    <t>D059B6N8</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>x_s</t>
+  </si>
+  <si>
+    <t>x_L</t>
+  </si>
+  <si>
+    <t>measd_lv</t>
+  </si>
+  <si>
+    <t>fabd</t>
+  </si>
+  <si>
+    <t>measd</t>
+  </si>
+  <si>
     <t>D059BBN1</t>
-  </si>
-  <si>
-    <t>D059BBN2_n</t>
-  </si>
-  <si>
-    <t>D059BBN8</t>
-  </si>
-  <si>
-    <t>D053N2</t>
-  </si>
-  <si>
-    <t>D053N4</t>
-  </si>
-  <si>
-    <t>D053N7</t>
-  </si>
-  <si>
-    <t>D055B1N2</t>
-  </si>
-  <si>
-    <t>D055B1N4</t>
-  </si>
-  <si>
-    <t>D055B1N5</t>
-  </si>
-  <si>
-    <t>D057B1N6</t>
-  </si>
-  <si>
-    <t>D057B1N7</t>
-  </si>
-  <si>
-    <t>D057B1N8</t>
-  </si>
-  <si>
-    <t>D057B1N9</t>
-  </si>
-  <si>
-    <t>D059B6N5</t>
-  </si>
-  <si>
-    <t>D059B6N7</t>
-  </si>
-  <si>
-    <t>D059B6N8</t>
-  </si>
-  <si>
-    <t>Fin</t>
-  </si>
-  <si>
-    <t>x_s</t>
-  </si>
-  <si>
-    <t>x_L</t>
-  </si>
-  <si>
-    <t>measd_lv</t>
-  </si>
-  <si>
-    <t>fabd</t>
-  </si>
-  <si>
-    <t>measd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,8 +201,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -245,6 +259,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -291,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,9 +345,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,6 +397,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,14 +590,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,18 +652,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2">
-        <v>0.000219</v>
+        <v>2.1900000000000001E-4</v>
       </c>
       <c r="C2">
         <v>121000</v>
       </c>
       <c r="D2">
-        <v>1.54e-10</v>
+        <v>1.5400000000000001E-10</v>
       </c>
       <c r="E2">
         <v>905000</v>
@@ -609,51 +672,51 @@
         <v>666800000</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2">
         <v>4033.333333333333</v>
       </c>
       <c r="M2">
-        <v>30166.66666666667</v>
+        <v>30166.666666666672</v>
       </c>
       <c r="N2">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O2">
         <v>1.679965774519973</v>
       </c>
       <c r="P2">
-        <v>7.047706305373377e-08</v>
+        <v>7.0477063053733765E-8</v>
       </c>
       <c r="Q2">
-        <v>1.58075307327616</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>1.5807530732761601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0001955</v>
+        <v>1.9550000000000001E-4</v>
       </c>
       <c r="C3">
         <v>90800</v>
       </c>
       <c r="D3">
-        <v>1.975e-09</v>
+        <v>1.9749999999999999E-9</v>
       </c>
       <c r="E3">
         <v>72600</v>
@@ -662,19 +725,19 @@
         <v>25910000</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3">
         <v>3026.666666666667</v>
@@ -683,30 +746,30 @@
         <v>2420</v>
       </c>
       <c r="N3">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O3">
         <v>2.238720910979259</v>
       </c>
       <c r="P3">
-        <v>9.391767213107694e-08</v>
+        <v>9.3917672131076941E-8</v>
       </c>
       <c r="Q3">
-        <v>1.824793795964304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>1.8247937959643039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4">
-        <v>3.2e-07</v>
+        <v>3.2000000000000001E-7</v>
       </c>
       <c r="C4">
         <v>9400</v>
       </c>
       <c r="D4">
-        <v>3.9e-09</v>
+        <v>3.9000000000000002E-9</v>
       </c>
       <c r="E4">
         <v>99.7</v>
@@ -721,13 +784,13 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4">
         <v>4700</v>
@@ -736,30 +799,30 @@
         <v>49.85</v>
       </c>
       <c r="N4">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O4">
         <v>1.441672756857566</v>
       </c>
       <c r="P4">
-        <v>6.048031652128927e-08</v>
+        <v>6.0480316521289266E-8</v>
       </c>
       <c r="Q4">
-        <v>1.464357661130454</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>1.4643576611304541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.001385</v>
+        <v>1.3849999999999999E-3</v>
       </c>
       <c r="C5">
         <v>1750000</v>
       </c>
       <c r="D5">
-        <v>3.2e-13</v>
+        <v>3.2E-13</v>
       </c>
       <c r="E5">
         <v>236700000</v>
@@ -774,13 +837,13 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L5">
         <v>87500</v>
@@ -789,30 +852,30 @@
         <v>11835000</v>
       </c>
       <c r="N5">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O5">
-        <v>0.07743842236834926</v>
+        <v>7.7438422368349261E-2</v>
       </c>
       <c r="P5">
-        <v>3.248657001714966e-09</v>
+        <v>3.248657001714966E-9</v>
       </c>
       <c r="Q5">
-        <v>0.339384548695241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>0.33938454869524098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0.002495</v>
+        <v>2.4949999999999998E-3</v>
       </c>
       <c r="C6">
         <v>993000</v>
       </c>
       <c r="D6">
-        <v>2.1e-11</v>
+        <v>2.0999999999999999E-11</v>
       </c>
       <c r="E6">
         <v>4319000</v>
@@ -827,13 +890,13 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L6">
         <v>49650</v>
@@ -842,30 +905,30 @@
         <v>215950</v>
       </c>
       <c r="N6">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O6">
-        <v>0.1364725469734251</v>
+        <v>0.13647254697342509</v>
       </c>
       <c r="P6">
-        <v>5.72522633736273e-09</v>
+        <v>5.7252263373627302E-9</v>
       </c>
       <c r="Q6">
-        <v>0.4505432279086851</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>0.45054322790868512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.003345</v>
+        <v>3.3449999999999999E-3</v>
       </c>
       <c r="C7">
         <v>664000</v>
       </c>
       <c r="D7">
-        <v>1.2e-12</v>
+        <v>1.1999999999999999E-12</v>
       </c>
       <c r="E7">
         <v>22920000</v>
@@ -880,13 +943,13 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L7">
         <v>33200</v>
@@ -895,30 +958,30 @@
         <v>1146000</v>
       </c>
       <c r="N7">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O7">
-        <v>0.2040922276274265</v>
+        <v>0.20409222762742649</v>
       </c>
       <c r="P7">
-        <v>8.561972519580107e-09</v>
+        <v>8.5619725195801066E-9</v>
       </c>
       <c r="Q7">
-        <v>0.5509688561444098</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>0.55096885614440982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8">
-        <v>0.0003186</v>
+        <v>3.1859999999999999E-4</v>
       </c>
       <c r="C8">
         <v>119000</v>
       </c>
       <c r="D8">
-        <v>2.68e-12</v>
+        <v>2.6799999999999999E-12</v>
       </c>
       <c r="E8">
         <v>29090000</v>
@@ -933,13 +996,13 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L8">
         <v>29750</v>
@@ -948,30 +1011,30 @@
         <v>7272500</v>
       </c>
       <c r="N8">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O8">
         <v>0.2277600657892625</v>
       </c>
       <c r="P8">
-        <v>9.554873534455783e-09</v>
+        <v>9.5548735344557828E-9</v>
       </c>
       <c r="Q8">
-        <v>0.5820396992046273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>0.58203969920462728</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="C9">
         <v>594000</v>
       </c>
       <c r="D9">
-        <v>2e-11</v>
+        <v>1.9999999999999999E-11</v>
       </c>
       <c r="E9">
         <v>7715000</v>
@@ -986,45 +1049,45 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J9">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L9">
         <v>19800</v>
       </c>
       <c r="M9">
-        <v>257166.6666666667</v>
+        <v>257166.66666666669</v>
       </c>
       <c r="N9">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O9">
-        <v>0.3422152503651797</v>
+        <v>0.34221525036517969</v>
       </c>
       <c r="P9">
-        <v>1.435643877020503e-08</v>
+        <v>1.4356438770205029E-8</v>
       </c>
       <c r="Q9">
-        <v>0.7134499264189915</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>0.71344992641899152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10">
-        <v>0.00307</v>
+        <v>3.0699999999999998E-3</v>
       </c>
       <c r="C10">
         <v>585000</v>
       </c>
       <c r="D10">
-        <v>2.2e-11</v>
+        <v>2.2000000000000002E-11</v>
       </c>
       <c r="E10">
         <v>265000</v>
@@ -1039,45 +1102,45 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10">
         <v>19500</v>
       </c>
       <c r="M10">
-        <v>8833.333333333334</v>
+        <v>8833.3333333333339</v>
       </c>
       <c r="N10">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O10">
-        <v>0.3474801003707979</v>
+        <v>0.34748010037079791</v>
       </c>
       <c r="P10">
-        <v>1.457730705897741e-08</v>
+        <v>1.4577307058977409E-8</v>
       </c>
       <c r="Q10">
-        <v>0.07939110757275286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>7.9391107572752861E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B11">
-        <v>0.00172</v>
+        <v>1.72E-3</v>
       </c>
       <c r="C11">
         <v>66100</v>
       </c>
       <c r="D11">
-        <v>5.4e-09</v>
+        <v>5.4000000000000004E-9</v>
       </c>
       <c r="E11">
         <v>851</v>
@@ -1092,34 +1155,34 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11">
         <v>2203.333333333333</v>
       </c>
       <c r="M11">
-        <v>28.36666666666667</v>
+        <v>28.366666666666671</v>
       </c>
       <c r="N11">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O11">
-        <v>3.075277741556986</v>
+        <v>3.0752777415569859</v>
       </c>
       <c r="P11">
-        <v>1.29012475484142e-07</v>
+        <v>1.29012475484142E-7</v>
       </c>
       <c r="Q11">
-        <v>2.138730142415677</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>2.1387301424156768</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1127,7 +1190,7 @@
         <v>168000</v>
       </c>
       <c r="D12">
-        <v>1.6e-10</v>
+        <v>1.5999999999999999E-10</v>
       </c>
       <c r="E12">
         <v>23730</v>
@@ -1139,13 +1202,13 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J12">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12">
         <v>11200</v>
@@ -1154,33 +1217,33 @@
         <v>1582</v>
       </c>
       <c r="N12">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O12">
-        <v>0.6049876747527285</v>
+        <v>0.60498767475272852</v>
       </c>
       <c r="P12">
-        <v>2.538013282589817e-08</v>
+        <v>2.538013282589817E-8</v>
       </c>
       <c r="Q12">
         <v>0.1047563010599542</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13">
-        <v>0.0001645</v>
+        <v>1.6449999999999999E-4</v>
       </c>
       <c r="C13">
         <v>1450</v>
       </c>
       <c r="D13">
-        <v>1.37e-07</v>
+        <v>1.37E-7</v>
       </c>
       <c r="E13">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1189,45 +1252,45 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13">
-        <v>3.74e-12</v>
+        <v>3.7399999999999998E-12</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13">
         <v>1450</v>
       </c>
       <c r="M13">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N13">
-        <v>0.002422982803154429</v>
+        <v>2.422982803154429E-3</v>
       </c>
       <c r="O13">
-        <v>4.673008246365902</v>
+        <v>4.6730082463659022</v>
       </c>
       <c r="P13">
-        <v>1.960396466552135e-07</v>
+        <v>1.9603964665521351E-7</v>
       </c>
       <c r="Q13">
-        <v>0.3009666907808027</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>0.30096669078080268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B14">
-        <v>0.002021</v>
+        <v>2.0209999999999998E-3</v>
       </c>
       <c r="C14">
         <v>23300</v>
       </c>
       <c r="D14">
-        <v>5.6e-09</v>
+        <v>5.5999999999999997E-9</v>
       </c>
       <c r="E14">
         <v>-307</v>
@@ -1239,45 +1302,45 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J14">
-        <v>3.74e-12</v>
+        <v>3.7399999999999998E-12</v>
       </c>
       <c r="K14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14">
         <v>1553.333333333333</v>
       </c>
       <c r="M14">
-        <v>-20.46666666666667</v>
+        <v>-20.466666666666669</v>
       </c>
       <c r="N14">
-        <v>0.002422982803154429</v>
+        <v>2.422982803154429E-3</v>
       </c>
       <c r="O14">
-        <v>4.362142890920961</v>
+        <v>4.3621428909209614</v>
       </c>
       <c r="P14">
-        <v>1.829983826073345e-07</v>
+        <v>1.829983826073345E-7</v>
       </c>
       <c r="Q14">
-        <v>0.2907837300758601</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>0.29078373007586011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B15">
-        <v>0.001972</v>
+        <v>1.9719999999999998E-3</v>
       </c>
       <c r="C15">
         <v>13500</v>
       </c>
       <c r="D15">
-        <v>9e-09</v>
+        <v>8.9999999999999995E-9</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1289,13 +1352,13 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J15">
-        <v>2.25e-12</v>
+        <v>2.2499999999999999E-12</v>
       </c>
       <c r="K15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L15">
         <v>1500</v>
@@ -1304,30 +1367,30 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="N15">
-        <v>0.00399838579370588</v>
+        <v>3.9983857937058798E-3</v>
       </c>
       <c r="O15">
-        <v>4.517241304820373</v>
+        <v>4.5172413048203728</v>
       </c>
       <c r="P15">
-        <v>1.895049917667064e-07</v>
+        <v>1.895049917667064E-7</v>
       </c>
       <c r="Q15">
-        <v>0.3801228586647764</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>0.38012285866477641</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16">
-        <v>0.001931</v>
+        <v>1.931E-3</v>
       </c>
       <c r="C16">
         <v>254000</v>
       </c>
       <c r="D16">
-        <v>3.71e-11</v>
+        <v>3.71E-11</v>
       </c>
       <c r="E16">
         <v>10000</v>
@@ -1339,45 +1402,45 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L16">
-        <v>16933.33333333333</v>
+        <v>16933.333333333328</v>
       </c>
       <c r="M16">
-        <v>666.6666666666666</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="N16">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O16">
-        <v>0.400149328182907</v>
+        <v>0.40014932818290699</v>
       </c>
       <c r="P16">
-        <v>1.678685950689328e-08</v>
+        <v>1.678685950689328E-8</v>
       </c>
       <c r="Q16">
-        <v>0.085195751409178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+        <v>8.5195751409177997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B17">
-        <v>9.685e-05</v>
+        <v>9.6849999999999996E-5</v>
       </c>
       <c r="C17">
         <v>16700</v>
       </c>
       <c r="D17">
-        <v>8e-10</v>
+        <v>8.0000000000000003E-10</v>
       </c>
       <c r="E17">
         <v>100000</v>
@@ -1389,13 +1452,13 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J17">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L17">
         <v>16700</v>
@@ -1404,339 +1467,339 @@
         <v>100000</v>
       </c>
       <c r="N17">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O17">
-        <v>0.4057402369599137</v>
+        <v>0.40574023695991368</v>
       </c>
       <c r="P17">
-        <v>1.702140644611135e-08</v>
+        <v>1.702140644611135E-8</v>
       </c>
       <c r="Q17">
-        <v>0.08578886673568814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+        <v>8.5788866735688141E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B18">
-        <v>1e-99</v>
+        <v>1E-99</v>
       </c>
       <c r="C18">
         <v>745000</v>
       </c>
       <c r="D18">
-        <v>6e-13</v>
+        <v>5.9999999999999997E-13</v>
       </c>
       <c r="E18">
         <v>240000000</v>
       </c>
       <c r="G18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18">
-        <v>24833.33333333333</v>
+        <v>24833.333333333328</v>
       </c>
       <c r="M18">
         <v>8000000</v>
       </c>
       <c r="N18">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O18">
-        <v>0.2728535016334454</v>
+        <v>0.27285350163344541</v>
       </c>
       <c r="P18">
-        <v>1.1446610240942e-08</v>
+        <v>1.1446610240942001E-8</v>
       </c>
       <c r="Q18">
-        <v>0.07035122392769246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>7.0351223927692455E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19">
-        <v>1e-99</v>
+        <v>1E-99</v>
       </c>
       <c r="C19">
         <v>1950000</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J19">
-        <v>2.25e-14</v>
+        <v>2.2499999999999999E-14</v>
       </c>
       <c r="K19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19">
         <v>65000</v>
       </c>
       <c r="N19">
-        <v>0.3098748990122057</v>
+        <v>0.30987489901220572</v>
       </c>
       <c r="O19">
-        <v>0.1042440301112394</v>
+        <v>0.10424403011123939</v>
       </c>
       <c r="P19">
-        <v>4.373192117693223e-09</v>
+        <v>4.3731921176932226E-9</v>
       </c>
       <c r="Q19">
-        <v>0.5083511251357323</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+        <v>0.50835112513573233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20">
-        <v>1e-99</v>
+        <v>1E-99</v>
       </c>
       <c r="C20">
         <v>1780000</v>
       </c>
       <c r="D20">
-        <v>7.5e-13</v>
+        <v>7.5000000000000004E-13</v>
       </c>
       <c r="E20">
         <v>50000000</v>
       </c>
       <c r="G20">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J20">
-        <v>4e-12</v>
+        <v>3.9999999999999999E-12</v>
       </c>
       <c r="K20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L20">
-        <v>59333.33333333334</v>
+        <v>59333.333333333343</v>
       </c>
       <c r="M20">
         <v>1666666.666666667</v>
       </c>
       <c r="N20">
-        <v>0.002267377309845408</v>
+        <v>2.2673773098454081E-3</v>
       </c>
       <c r="O20">
         <v>0.1141999206274813</v>
       </c>
       <c r="P20">
-        <v>4.790856533427969e-09</v>
+        <v>4.7908565334279686E-9</v>
       </c>
       <c r="Q20">
-        <v>0.04551345373112418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <v>4.5513453731124177E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21">
-        <v>0.00161</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="C21">
         <v>8900</v>
       </c>
       <c r="D21">
-        <v>9.06e-08</v>
+        <v>9.0600000000000004E-8</v>
       </c>
       <c r="E21">
         <v>734</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J21">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21">
-        <v>296.6666666666667</v>
+        <v>296.66666666666669</v>
       </c>
       <c r="M21">
-        <v>24.46666666666667</v>
+        <v>24.466666666666669</v>
       </c>
       <c r="N21">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O21">
-        <v>22.83998412549626</v>
+        <v>22.839984125496262</v>
       </c>
       <c r="P21">
-        <v>9.581713066855938e-07</v>
+        <v>9.5817130668559385E-7</v>
       </c>
       <c r="Q21">
         <v>5.828565974300794</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22">
-        <v>0.000353</v>
+        <v>3.5300000000000002E-4</v>
       </c>
       <c r="C22">
         <v>5300</v>
       </c>
       <c r="D22">
-        <v>2e-08</v>
+        <v>2E-8</v>
       </c>
       <c r="E22">
         <v>17700</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J22">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L22">
-        <v>176.6666666666667</v>
+        <v>176.66666666666671</v>
       </c>
       <c r="M22">
         <v>590</v>
       </c>
       <c r="N22">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O22">
-        <v>38.35393560696543</v>
+        <v>38.353935606965429</v>
       </c>
       <c r="P22">
-        <v>1.609004647075809e-06</v>
+        <v>1.609004647075809E-6</v>
       </c>
       <c r="Q22">
-        <v>7.552987834629382</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <v>7.5529878346293824</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23">
-        <v>0.000333</v>
+        <v>3.3300000000000002E-4</v>
       </c>
       <c r="C23">
         <v>10000</v>
       </c>
       <c r="D23">
-        <v>1e-08</v>
+        <v>1E-8</v>
       </c>
       <c r="E23">
         <v>33300</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L23">
-        <v>333.3333333333333</v>
+        <v>333.33333333333331</v>
       </c>
       <c r="M23">
         <v>1110</v>
       </c>
       <c r="N23">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O23">
-        <v>20.32758587169167</v>
+        <v>20.327585871691671</v>
       </c>
       <c r="P23">
-        <v>8.527724629501787e-07</v>
+        <v>8.5277246295017865E-7</v>
       </c>
       <c r="Q23">
-        <v>5.498658142850081</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+        <v>5.4986581428500809</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
-        <v>0.000219</v>
+        <v>2.1900000000000001E-4</v>
       </c>
       <c r="C24">
         <v>80100</v>
       </c>
       <c r="D24">
-        <v>1.1e-10</v>
+        <v>1.0999999999999999E-10</v>
       </c>
       <c r="E24">
         <v>558000</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L24">
         <v>2670</v>
@@ -1745,48 +1808,48 @@
         <v>18600</v>
       </c>
       <c r="N24">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O24">
         <v>2.53777601394403</v>
       </c>
       <c r="P24">
-        <v>1.064634785206216e-07</v>
+        <v>1.0646347852062161E-7</v>
       </c>
       <c r="Q24">
         <v>1.942855324766932</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
-        <v>0.00045</v>
+        <v>4.4999999999999999E-4</v>
       </c>
       <c r="C25">
         <v>157900</v>
       </c>
       <c r="D25">
-        <v>6.4e-11</v>
+        <v>6.3999999999999999E-11</v>
       </c>
       <c r="E25">
         <v>3588000</v>
       </c>
       <c r="G25">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J25">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L25">
         <v>5263.333333333333</v>
@@ -1795,183 +1858,183 @@
         <v>119600</v>
       </c>
       <c r="N25">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O25">
         <v>1.287370859511823</v>
       </c>
       <c r="P25">
-        <v>5.400712241609745e-08</v>
+        <v>5.4007122416097452E-8</v>
       </c>
       <c r="Q25">
-        <v>1.383775557088618</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+        <v>1.3837755570886181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <v>0.000103</v>
+        <v>1.03E-4</v>
       </c>
       <c r="C26">
         <v>108700</v>
       </c>
       <c r="D26">
-        <v>5.9e-11</v>
+        <v>5.9000000000000003E-11</v>
       </c>
       <c r="E26">
         <v>1282000</v>
       </c>
       <c r="G26">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J26">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L26">
         <v>3623.333333333333</v>
       </c>
       <c r="M26">
-        <v>42733.33333333334</v>
+        <v>42733.333333333343</v>
       </c>
       <c r="N26">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O26">
         <v>1.870063097671727</v>
       </c>
       <c r="P26">
-        <v>7.845192851427587e-08</v>
+        <v>7.8451928514275866E-8</v>
       </c>
       <c r="Q26">
-        <v>1.667792236754896</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>1.6677922367548961</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27">
-        <v>9.679999999999999e-05</v>
+        <v>9.6799999999999995E-5</v>
       </c>
       <c r="C27">
         <v>92400</v>
       </c>
       <c r="D27">
-        <v>7e-10</v>
+        <v>6.9999999999999996E-10</v>
       </c>
       <c r="E27">
         <v>114.5</v>
       </c>
       <c r="G27">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J27">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L27">
         <v>3080</v>
       </c>
       <c r="M27">
-        <v>3.816666666666667</v>
+        <v>3.8166666666666669</v>
       </c>
       <c r="N27">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O27">
-        <v>2.199955180919012</v>
+        <v>2.1999551809190119</v>
       </c>
       <c r="P27">
-        <v>9.229139209417518e-08</v>
+        <v>9.2291392094175183E-8</v>
       </c>
       <c r="Q27">
-        <v>1.808925722546273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+        <v>1.8089257225462729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
-        <v>6.8e-05</v>
+        <v>6.7999999999999999E-5</v>
       </c>
       <c r="D28">
-        <v>7e-10</v>
+        <v>6.9999999999999996E-10</v>
       </c>
       <c r="E28">
         <v>123500</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H28">
         <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J28">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M28">
         <v>4116.666666666667</v>
       </c>
       <c r="N28">
-        <v>0.1859249394073234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>0.18592493940732341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29">
-        <v>0.0003065</v>
+        <v>3.0650000000000002E-4</v>
       </c>
       <c r="C29">
         <v>157900</v>
       </c>
       <c r="D29">
-        <v>2.55e-09</v>
+        <v>2.5500000000000001E-9</v>
       </c>
       <c r="E29">
         <v>112200</v>
       </c>
       <c r="G29">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H29">
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J29">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L29">
         <v>5263.333333333333</v>
@@ -1980,83 +2043,83 @@
         <v>3740</v>
       </c>
       <c r="N29">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O29">
         <v>1.287370859511823</v>
       </c>
       <c r="P29">
-        <v>5.400712241609745e-08</v>
+        <v>5.4007122416097452E-8</v>
       </c>
       <c r="Q29">
-        <v>1.383775557088618</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>1.3837755570886181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30">
-        <v>0.0001345</v>
+        <v>1.3449999999999999E-4</v>
       </c>
       <c r="D30">
-        <v>5.75e-10</v>
+        <v>5.7499999999999998E-10</v>
       </c>
       <c r="E30">
         <v>206000</v>
       </c>
       <c r="G30">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M30">
         <v>6866.666666666667</v>
       </c>
       <c r="N30">
-        <v>0.1859249394073234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>0.18592493940732341</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31">
-        <v>0.000133</v>
+        <v>1.3300000000000001E-4</v>
       </c>
       <c r="C31">
         <v>86200</v>
       </c>
       <c r="D31">
-        <v>1.45e-09</v>
+        <v>1.45E-9</v>
       </c>
       <c r="E31">
         <v>80350</v>
       </c>
       <c r="G31">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J31">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L31">
         <v>2873.333333333333</v>
@@ -2065,48 +2128,48 @@
         <v>2678.333333333333</v>
       </c>
       <c r="N31">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O31">
-        <v>2.358188616205531</v>
+        <v>2.3581886162055312</v>
       </c>
       <c r="P31">
-        <v>9.892952006382582e-08</v>
+        <v>9.8929520063825818E-8</v>
       </c>
       <c r="Q31">
         <v>1.872850395688995</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32">
-        <v>0.0001732</v>
+        <v>1.7320000000000001E-4</v>
       </c>
       <c r="C32">
         <v>78000</v>
       </c>
       <c r="D32">
-        <v>1.8e-09</v>
+        <v>1.8E-9</v>
       </c>
       <c r="E32">
         <v>80900</v>
       </c>
       <c r="G32">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32">
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L32">
         <v>2600</v>
@@ -2115,48 +2178,48 @@
         <v>2696.666666666667</v>
       </c>
       <c r="N32">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O32">
-        <v>2.606100752780984</v>
+        <v>2.6061007527809839</v>
       </c>
       <c r="P32">
-        <v>1.093298029423306e-07</v>
+        <v>1.093298029423306E-7</v>
       </c>
       <c r="Q32">
-        <v>1.968835441676494</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <v>1.9688354416764939</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33">
-        <v>0.0001624</v>
+        <v>1.6239999999999999E-4</v>
       </c>
       <c r="C33">
         <v>88100</v>
       </c>
       <c r="D33">
-        <v>1.575e-09</v>
+        <v>1.575E-9</v>
       </c>
       <c r="E33">
         <v>65900</v>
       </c>
       <c r="G33">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J33">
-        <v>4e-14</v>
+        <v>4E-14</v>
       </c>
       <c r="K33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L33">
         <v>2936.666666666667</v>
@@ -2165,19 +2228,21 @@
         <v>2196.666666666667</v>
       </c>
       <c r="N33">
-        <v>0.1859249394073234</v>
+        <v>0.18592493940732341</v>
       </c>
       <c r="O33">
-        <v>2.307330972950247</v>
+        <v>2.3073309729502469</v>
       </c>
       <c r="P33">
-        <v>9.679596628265365e-08</v>
+        <v>9.6795966282653648E-8</v>
       </c>
       <c r="Q33">
         <v>1.852544998294865</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>